<commit_message>
Added new product with same name & id but different batch number and inventory id
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inventory Management\pos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643B9FE4-23D0-4236-8FC6-26D153ECE037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46394CF-ECF4-413B-899A-62737EE11871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AEFF70B0-5DC5-4675-91F4-4F9BEC3F244F}"/>
   </bookViews>
@@ -488,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F026D6D2-5D6E-4A23-9A7E-054E052785D8}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +499,7 @@
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -509,8 +509,11 @@
       <c r="C1">
         <v>297</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -520,8 +523,11 @@
       <c r="C2">
         <v>315</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -531,8 +537,11 @@
       <c r="C3">
         <v>480</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -542,8 +551,11 @@
       <c r="C4">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -553,8 +565,11 @@
       <c r="C5">
         <v>190</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -564,8 +579,11 @@
       <c r="C6">
         <v>275</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -575,8 +593,11 @@
       <c r="C7">
         <v>350</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -586,8 +607,11 @@
       <c r="C8">
         <v>198</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,8 +621,11 @@
       <c r="C9">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -608,8 +635,11 @@
       <c r="C10">
         <v>180</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -619,8 +649,11 @@
       <c r="C11">
         <v>240</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -630,8 +663,11 @@
       <c r="C12">
         <v>360</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -641,8 +677,11 @@
       <c r="C13">
         <v>279</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -652,8 +691,11 @@
       <c r="C14">
         <v>170</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -662,6 +704,9 @@
       </c>
       <c r="C15">
         <v>225</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>